<commit_message>
Adjusted total time and dx to make figure work properly
</commit_message>
<xml_diff>
--- a/velocity_data.xlsx
+++ b/velocity_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadia/Downloads/NumericalModeling/Homework/finalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD166E6C-3DB4-FE46-8D11-4E8773CC53DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C38CBFD4-ADD0-194E-AC2B-9F300A055593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="780" windowWidth="27640" windowHeight="15760" xr2:uid="{869524EC-54AB-B74B-A3F1-DC4D754848F3}"/>
+    <workbookView xWindow="6980" yWindow="760" windowWidth="27640" windowHeight="15760" xr2:uid="{869524EC-54AB-B74B-A3F1-DC4D754848F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Site Number</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Distance from x-1</t>
+  </si>
+  <si>
+    <t>Velocity in km/s</t>
   </si>
 </sst>
 </file>
@@ -80,8 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40070BE-8B1C-5D49-B1E3-2D122D948473}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +418,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>7091200</v>
       </c>
@@ -425,8 +432,15 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f>B2*0.0003048*1000</f>
+        <v>0.68924313052799979</v>
+      </c>
+      <c r="E2">
+        <v>0.6892431</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>7094500</v>
       </c>
@@ -436,8 +450,15 @@
       <c r="C3">
         <v>60.433</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">B3*0.0003048*1000</f>
+        <v>1.1359363453439999</v>
+      </c>
+      <c r="E3">
+        <v>1.1359399999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>7099973</v>
       </c>
@@ -447,8 +468,15 @@
       <c r="C4">
         <v>73.430000000000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>3.4021273079999997E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3.4021000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>7109500</v>
       </c>
@@ -458,8 +486,15 @@
       <c r="C5">
         <v>16.77</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.4945333152239999</v>
+      </c>
+      <c r="E5">
+        <v>0.49453000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7124000</v>
       </c>
@@ -469,8 +504,15 @@
       <c r="C6">
         <v>103.16</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.23742788582399998</v>
+      </c>
+      <c r="E6">
+        <v>0.23743</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7130500</v>
       </c>
@@ -480,8 +522,15 @@
       <c r="C7">
         <v>25.77</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.59842784860799991</v>
+      </c>
+      <c r="E7">
+        <v>0.59843000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7133000</v>
       </c>
@@ -491,8 +540,15 @@
       <c r="C8">
         <v>30.699000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.30000455111999996</v>
+      </c>
+      <c r="E8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7134180</v>
       </c>
@@ -502,8 +558,15 @@
       <c r="C9">
         <v>26.286999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.17721242688</v>
+      </c>
+      <c r="E9">
+        <v>0.17721000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7135500</v>
       </c>
@@ -513,13 +576,20 @@
       <c r="C10">
         <v>18.042999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.134091752136</v>
+      </c>
+      <c r="E10">
+        <v>0.13408999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>7.8712900000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13">
         <f>SUM(C3:C11)</f>
         <v>362.46328999999997</v>

</xml_diff>

<commit_message>
Updated Excel spreadsheet to be more user-friendly.
</commit_message>
<xml_diff>
--- a/velocity_data.xlsx
+++ b/velocity_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadia/Downloads/NumericalModeling/Homework/finalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C38CBFD4-ADD0-194E-AC2B-9F300A055593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAE01A34-404B-3648-931E-1B2C709D3036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="760" windowWidth="27640" windowHeight="15760" xr2:uid="{869524EC-54AB-B74B-A3F1-DC4D754848F3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{869524EC-54AB-B74B-A3F1-DC4D754848F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Site Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Velocity </t>
-  </si>
-  <si>
-    <t>Distance from x-1</t>
-  </si>
-  <si>
-    <t>Velocity in km/s</t>
+    <t>Parkdale</t>
+  </si>
+  <si>
+    <t>Pueblo</t>
+  </si>
+  <si>
+    <t>Las Animas</t>
+  </si>
+  <si>
+    <t>Lamar</t>
+  </si>
+  <si>
+    <t>Velocity (ft/s)</t>
+  </si>
+  <si>
+    <t>Distance from x-1 (m)</t>
+  </si>
+  <si>
+    <t>Velocity in m/s</t>
+  </si>
+  <si>
+    <t>5.3125, 79.42</t>
+  </si>
+  <si>
+    <t>4.1575, 74.25</t>
+  </si>
+  <si>
+    <t>2.765, 143.27</t>
+  </si>
+  <si>
+    <t>5.21, 146.48</t>
+  </si>
+  <si>
+    <t>8.6325, 48.79</t>
+  </si>
+  <si>
+    <t>2.1075, 112.11</t>
+  </si>
+  <si>
+    <t>6.453333, 29.96</t>
+  </si>
+  <si>
+    <t>6.366, 54.83</t>
+  </si>
+  <si>
+    <t>14.2775, 37.05</t>
+  </si>
+  <si>
+    <t>USGS Gauge Height, GoogleEarth River width (ft)</t>
+  </si>
+  <si>
+    <t>USGS Average Spring Discharge (ft^3/s)</t>
+  </si>
+  <si>
+    <t>Neighboring Cities</t>
   </si>
 </sst>
 </file>
@@ -63,12 +111,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,9 +137,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,200 +462,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40070BE-8B1C-5D49-B1E3-2D122D948473}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>954.08333000000005</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.2612963599999998</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.6892431</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1">
+        <v>7091200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>60.433</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1150.45</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.7268252799999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.1359399999999999</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G3" s="1">
+        <v>7094500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>73.430000000000007</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44.216666699999998</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.11161835000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.4021000000000003E-2</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G4" s="1">
+        <v>7099973</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>16.77</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1238.21667</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.62248463</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.49453000000000003</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <v>7109500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>103.16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
+        <v>328.08333299999998</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.77896288000000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.23743</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>7091200</v>
-      </c>
-      <c r="B2">
-        <v>2.2612963599999998</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <f>B2*0.0003048*1000</f>
-        <v>0.68924313052799979</v>
-      </c>
-      <c r="E2">
-        <v>0.6892431</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>7094500</v>
-      </c>
-      <c r="B3">
-        <v>3.7268252799999999</v>
-      </c>
-      <c r="C3">
-        <v>60.433</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D10" si="0">B3*0.0003048*1000</f>
-        <v>1.1359363453439999</v>
-      </c>
-      <c r="E3">
-        <v>1.1359399999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>7099973</v>
-      </c>
-      <c r="B4">
-        <v>0.11161835000000001</v>
-      </c>
-      <c r="C4">
-        <v>73.430000000000007</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>3.4021273079999997E-2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3.4021000000000003E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>7109500</v>
-      </c>
-      <c r="B5">
-        <v>1.62248463</v>
-      </c>
-      <c r="C5">
-        <v>16.77</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.4945333152239999</v>
-      </c>
-      <c r="E5">
-        <v>0.49453000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="G6" s="1">
         <v>7124000</v>
       </c>
-      <c r="B6">
-        <v>0.77896288000000002</v>
-      </c>
-      <c r="C6">
-        <v>103.16</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0.23742788582399998</v>
-      </c>
-      <c r="E6">
-        <v>0.23743</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>25.77</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1">
+        <v>463.88333299999999</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.9633459600000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.59843000000000002</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
         <v>7130500</v>
       </c>
-      <c r="B7">
-        <v>1.9633459600000001</v>
-      </c>
-      <c r="C7">
-        <v>25.77</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0.59842784860799991</v>
-      </c>
-      <c r="E7">
-        <v>0.59843000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>30.699000000000002</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1">
+        <v>190.3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.98426689999999994</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
         <v>7133000</v>
       </c>
-      <c r="B8">
-        <v>0.98426689999999994</v>
-      </c>
-      <c r="C8">
-        <v>30.699000000000002</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0.30000455111999996</v>
-      </c>
-      <c r="E8">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>26.286999999999999</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1">
+        <v>202.938333</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.58140559999999997</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.17721000000000001</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
         <v>7134180</v>
       </c>
-      <c r="B9">
-        <v>0.58140559999999997</v>
-      </c>
-      <c r="C9">
-        <v>26.286999999999999</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0.17721242688</v>
-      </c>
-      <c r="E9">
-        <v>0.17721000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>18.042999999999999</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1">
+        <v>232.716667</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.43993357</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.13408999999999999</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
         <v>7135500</v>
       </c>
-      <c r="B10">
-        <v>0.43993357</v>
-      </c>
-      <c r="C10">
-        <v>18.042999999999999</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0.134091752136</v>
-      </c>
-      <c r="E10">
-        <v>0.13408999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>7.8712900000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C13">
-        <f>SUM(C3:C11)</f>
-        <v>362.46328999999997</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>